<commit_message>
change pid function,change ui
</commit_message>
<xml_diff>
--- a/FWG1_220/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/FWG1_220/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-6549d2.o</t>
+    <t>lto-llvm-a2ddd2.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -32,15 +32,15 @@
     <t>dadd.o</t>
   </si>
   <si>
+    <t>mc_w.l</t>
+  </si>
+  <si>
     <t>dmul.o</t>
   </si>
   <si>
     <t>ddiv.o</t>
   </si>
   <si>
-    <t>mc_w.l</t>
-  </si>
-  <si>
     <t>depilogue.o</t>
   </si>
   <si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>fmul.o</t>
+  </si>
+  <si>
+    <t>uldiv.o</t>
   </si>
   <si>
     <t>dfixi.o</t>
@@ -233,16 +236,16 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$35</c:f>
+              <c:f>ram_percent!$A$3:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-6549d2.o</c:v>
+                  <c:v>lto-llvm-a2ddd2.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -250,17 +253,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$35</c:f>
+              <c:f>ram_percent!$B$3:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>86.61175537109375</c:v>
+                  <c:v>92.87701416015625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.38824653625488</c:v>
-                </c:pt>
-                <c:pt idx="32">
+                  <c:v>7.122982978820801</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -328,11 +331,11 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$35</c:f>
+              <c:f>flash_percent!$A$3:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-6549d2.o</c:v>
+                  <c:v>lto-llvm-a2ddd2.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>mf_w.l</c:v>
@@ -344,13 +347,13 @@
                   <c:v>dadd.o</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>mc_w.l</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dmul.o</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>ddiv.o</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>mc_w.l</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>depilogue.o</c:v>
@@ -368,66 +371,69 @@
                   <c:v>fmul.o</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>uldiv.o</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>dfixi.o</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>dfixui.o</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>ffixui.o</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>memseta.o</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>llsshr.o</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>init.o</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>dflti.o</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>llushr.o</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>llshl.o</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>handlers.o</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>fcmplt.o</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>fcmple.o</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>fcmpgt.o</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>fcmpge.o</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>dfltui.o</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>fflti.o</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>ffltui.o</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>entry9a.o</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>entry2.o</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>entry5.o</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -435,107 +441,110 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$35</c:f>
+              <c:f>flash_percent!$B$3:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>89.45817565917969</c:v>
+                  <c:v>95.65807342529297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.284077167510986</c:v>
+                  <c:v>1.690988421440125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.94474196434021</c:v>
+                  <c:v>0.37290358543396</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7810490131378174</c:v>
+                  <c:v>0.3082915544509888</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5331711769104004</c:v>
+                  <c:v>0.2935231029987335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.519140362739563</c:v>
+                  <c:v>0.2104505300521851</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5144634246826172</c:v>
+                  <c:v>0.2049123644828796</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4349554479122162</c:v>
+                  <c:v>0.1716833263635635</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.4115707576274872</c:v>
+                  <c:v>0.1624530404806137</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2899703085422516</c:v>
+                  <c:v>0.1144555509090424</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2572317123413086</c:v>
+                  <c:v>0.1015331521630287</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2338470220565796</c:v>
+                  <c:v>0.09230286628007889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1449851542711258</c:v>
+                  <c:v>0.09045680612325668</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1169235110282898</c:v>
+                  <c:v>0.05722777545452118</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0935388058423996</c:v>
+                  <c:v>0.04615143314003944</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.084184929728508</c:v>
+                  <c:v>0.03692114725708962</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.084184929728508</c:v>
+                  <c:v>0.0332290306687355</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.084184929728508</c:v>
+                  <c:v>0.0332290306687355</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0795079842209816</c:v>
+                  <c:v>0.0332290306687355</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0748310461640358</c:v>
+                  <c:v>0.0313829742372036</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.07015410810709</c:v>
+                  <c:v>0.02953691594302654</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.07015410810709</c:v>
+                  <c:v>0.02769085951149464</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0654771625995636</c:v>
+                  <c:v>0.02769085951149464</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0654771625995636</c:v>
+                  <c:v>0.02584480121731758</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0654771625995636</c:v>
+                  <c:v>0.02584480121731758</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0654771625995636</c:v>
+                  <c:v>0.02584480121731758</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0608002245426178</c:v>
+                  <c:v>0.02584480121731758</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.042092464864254</c:v>
+                  <c:v>0.02399874478578568</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0233847014605999</c:v>
+                  <c:v>0.01661451533436775</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.01870776154100895</c:v>
+                  <c:v>0.009230286814272404</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.01870776154100895</c:v>
+                  <c:v>0.007384228985756636</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.009353880770504475</c:v>
+                  <c:v>0.007384228985756636</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>0.003692114492878318</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -640,8 +649,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H35" totalsRowCount="1">
-  <autoFilter ref="A2:H34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H36" totalsRowCount="1">
+  <autoFilter ref="A2:H35"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -657,8 +666,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H35" totalsRowCount="1">
-  <autoFilter ref="A2:H34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H36" totalsRowCount="1">
+  <autoFilter ref="A2:H35"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -958,7 +967,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -974,28 +983,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1003,25 +1012,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>86.61175537109375</v>
+        <v>92.87701416015625</v>
       </c>
       <c r="C3" s="1">
-        <v>13249</v>
+        <v>13352</v>
       </c>
       <c r="D3" s="1">
-        <v>38255</v>
+        <v>103635</v>
       </c>
       <c r="E3" s="1">
-        <v>37974</v>
+        <v>103324</v>
       </c>
       <c r="F3" s="1">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G3" s="1">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="H3" s="1">
-        <v>13116</v>
+        <v>13184</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1029,10 +1038,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>13.38824653625488</v>
+        <v>7.122982978820801</v>
       </c>
       <c r="C4" s="1">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="D4" s="1">
         <v>404</v>
@@ -1047,38 +1056,38 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1094,7 +1103,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1110,28 +1119,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1139,25 +1148,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>89.45817565917969</v>
+        <v>95.65807342529297</v>
       </c>
       <c r="C3" s="1">
-        <v>38255</v>
+        <v>103635</v>
       </c>
       <c r="D3" s="1">
-        <v>13249</v>
+        <v>13352</v>
       </c>
       <c r="E3" s="1">
-        <v>37974</v>
+        <v>103324</v>
       </c>
       <c r="F3" s="1">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G3" s="1">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="H3" s="1">
-        <v>13116</v>
+        <v>13184</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1165,7 +1174,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>4.284077167510986</v>
+        <v>1.690988421440125</v>
       </c>
       <c r="C4" s="1">
         <v>1832</v>
@@ -1191,13 +1200,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>0.94474196434021</v>
+        <v>0.37290358543396</v>
       </c>
       <c r="C5" s="1">
         <v>404</v>
       </c>
       <c r="D5" s="1">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="E5" s="1">
         <v>36</v>
@@ -1209,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>2048</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1217,7 +1226,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>0.7810490131378174</v>
+        <v>0.3082915544509888</v>
       </c>
       <c r="C6" s="1">
         <v>334</v>
@@ -1243,16 +1252,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>0.5331711769104004</v>
+        <v>0.2935231029987335</v>
       </c>
       <c r="C7" s="1">
-        <v>228</v>
+        <v>318</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>228</v>
+        <v>318</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1269,16 +1278,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>0.519140362739563</v>
+        <v>0.2104505300521851</v>
       </c>
       <c r="C8" s="1">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -1295,16 +1304,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>0.5144634246826172</v>
+        <v>0.2049123644828796</v>
       </c>
       <c r="C9" s="1">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1321,7 +1330,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>0.4349554479122162</v>
+        <v>0.1716833263635635</v>
       </c>
       <c r="C10" s="1">
         <v>186</v>
@@ -1347,7 +1356,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>0.4115707576274872</v>
+        <v>0.1624530404806137</v>
       </c>
       <c r="C11" s="1">
         <v>176</v>
@@ -1373,7 +1382,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>0.2899703085422516</v>
+        <v>0.1144555509090424</v>
       </c>
       <c r="C12" s="1">
         <v>124</v>
@@ -1399,7 +1408,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>0.2572317123413086</v>
+        <v>0.1015331521630287</v>
       </c>
       <c r="C13" s="1">
         <v>110</v>
@@ -1425,7 +1434,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>0.2338470220565796</v>
+        <v>0.09230286628007889</v>
       </c>
       <c r="C14" s="1">
         <v>100</v>
@@ -1451,16 +1460,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>0.1449851542711258</v>
+        <v>0.09045680612325668</v>
       </c>
       <c r="C15" s="1">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1477,16 +1486,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>0.1169235110282898</v>
+        <v>0.05722777545452118</v>
       </c>
       <c r="C16" s="1">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1503,16 +1512,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>0.0935388058423996</v>
+        <v>0.04615143314003944</v>
       </c>
       <c r="C17" s="1">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1529,16 +1538,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>0.084184929728508</v>
+        <v>0.03692114725708962</v>
       </c>
       <c r="C18" s="1">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -1555,7 +1564,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>0.084184929728508</v>
+        <v>0.0332290306687355</v>
       </c>
       <c r="C19" s="1">
         <v>36</v>
@@ -1581,7 +1590,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>0.084184929728508</v>
+        <v>0.0332290306687355</v>
       </c>
       <c r="C20" s="1">
         <v>36</v>
@@ -1607,16 +1616,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>0.0795079842209816</v>
+        <v>0.0332290306687355</v>
       </c>
       <c r="C21" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1633,16 +1642,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>0.0748310461640358</v>
+        <v>0.0313829742372036</v>
       </c>
       <c r="C22" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1659,16 +1668,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>0.07015410810709</v>
+        <v>0.02953691594302654</v>
       </c>
       <c r="C23" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1685,7 +1694,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>0.07015410810709</v>
+        <v>0.02769085951149464</v>
       </c>
       <c r="C24" s="1">
         <v>30</v>
@@ -1711,16 +1720,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>0.0654771625995636</v>
+        <v>0.02769085951149464</v>
       </c>
       <c r="C25" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -1737,7 +1746,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>0.0654771625995636</v>
+        <v>0.02584480121731758</v>
       </c>
       <c r="C26" s="1">
         <v>28</v>
@@ -1763,7 +1772,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2">
-        <v>0.0654771625995636</v>
+        <v>0.02584480121731758</v>
       </c>
       <c r="C27" s="1">
         <v>28</v>
@@ -1789,7 +1798,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2">
-        <v>0.0654771625995636</v>
+        <v>0.02584480121731758</v>
       </c>
       <c r="C28" s="1">
         <v>28</v>
@@ -1815,16 +1824,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>0.0608002245426178</v>
+        <v>0.02584480121731758</v>
       </c>
       <c r="C29" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -1841,16 +1850,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="2">
-        <v>0.042092464864254</v>
+        <v>0.02399874478578568</v>
       </c>
       <c r="C30" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -1867,16 +1876,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="2">
-        <v>0.0233847014605999</v>
+        <v>0.01661451533436775</v>
       </c>
       <c r="C31" s="1">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -1893,16 +1902,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="2">
-        <v>0.01870776154100895</v>
+        <v>0.009230286814272404</v>
       </c>
       <c r="C32" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -1919,7 +1928,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2">
-        <v>0.01870776154100895</v>
+        <v>0.007384228985756636</v>
       </c>
       <c r="C33" s="1">
         <v>8</v>
@@ -1945,56 +1954,82 @@
         <v>32</v>
       </c>
       <c r="B34" s="2">
-        <v>0.009353880770504475</v>
+        <v>0.007384228985756636</v>
       </c>
       <c r="C34" s="1">
+        <v>8</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>8</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.003692114492878318</v>
+      </c>
+      <c r="C35" s="1">
         <v>4</v>
       </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
         <v>4</v>
       </c>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
-      <c r="H34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35">
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>